<commit_message>
Changes in the tests to accomodate the new slice option in the single crystal tab
</commit_message>
<xml_diff>
--- a/Examples/Experiment/AlN/results.ref.xlsx
+++ b/Examples/Experiment/AlN/results.ref.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="84">
   <si>
     <t>Directory</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Single crystal</t>
+  </si>
+  <si>
+    <t>Slice thickness</t>
+  </si>
+  <si>
+    <t>Slice thickness unit</t>
   </si>
   <si>
     <t>Substrate</t>
@@ -817,13 +823,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3655,25 +3661,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -8917,25 +8923,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -15020,7 +15026,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H58"/>
+  <dimension ref="A2:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15258,8 +15264,8 @@
       <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
-        <v>64</v>
+      <c r="C20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -15267,10 +15273,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21">
-        <v>99999</v>
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -15278,13 +15284,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
         <v>66</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -15294,8 +15297,8 @@
       <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s">
-        <v>64</v>
+      <c r="C23">
+        <v>99999</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -15305,8 +15308,11 @@
       <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
-        <v>69</v>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -15314,10 +15320,10 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25">
-        <v>99999</v>
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -15325,40 +15331,34 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
         <v>71</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
         <v>1</v>
       </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
       <c r="C27">
-        <v>2.668224269059857</v>
-      </c>
-      <c r="D27">
-        <v>-1.5405</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
+        <v>99999</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
         <v>1</v>
       </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>3.081</v>
-      </c>
-      <c r="E28">
         <v>0</v>
       </c>
     </row>
@@ -15367,32 +15367,41 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>2.668224269059857</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>-1.5405</v>
       </c>
       <c r="E29">
-        <v>5.030999999999999</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>3.081</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32">
-        <v>7.2</v>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>5.030999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -15400,10 +15409,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -15411,10 +15417,10 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -15422,10 +15428,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -15433,10 +15439,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -15444,13 +15450,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -15458,13 +15461,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -15472,25 +15472,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -15498,13 +15486,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -15512,13 +15500,25 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -15526,13 +15526,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42">
-        <v>0.24</v>
-      </c>
-      <c r="D42">
-        <v>0.5600000000000001</v>
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -15540,10 +15540,13 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>51</v>
+      </c>
+      <c r="D43" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -15551,10 +15554,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="C44">
+        <v>0.24</v>
+      </c>
+      <c r="D44">
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -15562,10 +15568,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -15573,10 +15579,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -15584,10 +15590,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -15595,10 +15601,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -15606,10 +15612,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" t="s">
-        <v>74</v>
+        <v>60</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -15617,10 +15623,10 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50">
-        <v>99999</v>
+        <v>61</v>
+      </c>
+      <c r="C50" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -15628,12 +15634,9 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C51">
-        <v>11.6964</v>
-      </c>
-      <c r="D51">
         <v>0</v>
       </c>
     </row>
@@ -15642,10 +15645,10 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -15653,10 +15656,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -15664,7 +15667,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C54">
         <v>99999</v>
@@ -15675,10 +15678,10 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>11.6964</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -15688,41 +15691,88 @@
       <c r="A56">
         <v>1</v>
       </c>
-      <c r="C56">
-        <v>2.668224269059857</v>
-      </c>
-      <c r="D56">
-        <v>-1.5405</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
+      <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57">
         <v>1</v>
       </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>3.081</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58">
         <v>1</v>
       </c>
+      <c r="B58" t="s">
+        <v>72</v>
+      </c>
       <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>2.668224269059857</v>
+      </c>
+      <c r="D60">
+        <v>-1.5405</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>3.081</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
         <v>5.030999999999999</v>
       </c>
     </row>
@@ -15741,13 +15791,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -18579,13 +18629,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -21417,13 +21467,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -24255,13 +24305,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -27093,13 +27143,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>